<commit_message>
add some unit test.
</commit_message>
<xml_diff>
--- a/FireflySoft.Excel.UnitTest/file/data.xlsx
+++ b/FireflySoft.Excel.UnitTest/file/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>本科</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,10 +51,6 @@
   </si>
   <si>
     <t>李四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>女</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -74,6 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0_ "/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,10 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -427,7 +423,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -457,34 +453,34 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" s="3">
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>30912</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
       </c>
       <c r="C3" s="2">
         <v>30828</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>